<commit_message>
werkende metingen zonder storing voor 25 min lang
</commit_message>
<xml_diff>
--- a/docs/Rhea Hau 0850154 - Strookplanning 20181112.xlsx
+++ b/docs/Rhea Hau 0850154 - Strookplanning 20181112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RheaH\OneDrive\Afstudeerstage\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{946354C8-04F2-4C98-B374-6D2FBEF85EBA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{91A52452-80D0-4D75-84EE-A3FA264DF65C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -542,7 +542,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="49">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -763,6 +763,72 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFFFE699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor rgb="FFFFE699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor rgb="FFBCE4D1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor rgb="FFDBF1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor rgb="FF68C296"/>
       </patternFill>
     </fill>
   </fills>
@@ -1064,7 +1130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1371,61 +1437,6 @@
     <xf numFmtId="0" fontId="9" fillId="25" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1435,10 +1446,134 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="38" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="39" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="40" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="41" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="43" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="44" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="45" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="44" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="45" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="44" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="44" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="45" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="42" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="46" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="47" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="47" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="48" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="47" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1798,8 +1933,8 @@
   </sheetPr>
   <dimension ref="A1:DO1013"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B21" zoomScale="80" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AL8" zoomScale="80" workbookViewId="0">
+      <selection activeCell="CK17" sqref="CK17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1812,8 +1947,14 @@
     <col min="6" max="6" width="11.5546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="93" width="3.33203125" style="2" customWidth="1"/>
-    <col min="94" max="119" width="3" style="2" customWidth="1"/>
+    <col min="9" max="87" width="3.33203125" style="2" customWidth="1"/>
+    <col min="88" max="88" width="3.33203125" style="176" customWidth="1"/>
+    <col min="89" max="89" width="3.33203125" style="164" customWidth="1"/>
+    <col min="90" max="93" width="3.33203125" style="2" customWidth="1"/>
+    <col min="94" max="94" width="3" style="164" customWidth="1"/>
+    <col min="95" max="97" width="3" style="2" customWidth="1"/>
+    <col min="98" max="98" width="3" style="176" customWidth="1"/>
+    <col min="99" max="119" width="3" style="2" customWidth="1"/>
     <col min="120" max="16384" width="17.33203125" style="2"/>
   </cols>
   <sheetData>
@@ -1905,17 +2046,17 @@
       <c r="CG1" s="1"/>
       <c r="CH1" s="1"/>
       <c r="CI1" s="1"/>
-      <c r="CJ1" s="1"/>
-      <c r="CK1" s="1"/>
+      <c r="CJ1" s="165"/>
+      <c r="CK1" s="154"/>
       <c r="CL1" s="1"/>
       <c r="CM1" s="1"/>
       <c r="CN1" s="1"/>
       <c r="CO1" s="1"/>
-      <c r="CP1" s="1"/>
+      <c r="CP1" s="154"/>
       <c r="CQ1" s="1"/>
       <c r="CR1" s="1"/>
       <c r="CS1" s="1"/>
-      <c r="CT1" s="1"/>
+      <c r="CT1" s="165"/>
       <c r="CU1" s="1"/>
       <c r="CV1" s="1"/>
       <c r="CW1" s="1"/>
@@ -1977,23 +2118,23 @@
       <c r="AF2" s="103"/>
       <c r="AG2" s="103"/>
       <c r="AH2" s="103"/>
-      <c r="AI2" s="122" t="str">
+      <c r="AI2" s="144" t="str">
         <f>HYPERLINK("https://goo.gl/L6X1St","https://goo.gl/L6X1St")</f>
         <v>https://goo.gl/L6X1St</v>
       </c>
-      <c r="AJ2" s="123"/>
-      <c r="AK2" s="123"/>
-      <c r="AL2" s="123"/>
-      <c r="AM2" s="123"/>
-      <c r="AN2" s="123"/>
-      <c r="AO2" s="123"/>
-      <c r="AP2" s="123"/>
-      <c r="AQ2" s="123"/>
-      <c r="AR2" s="123"/>
-      <c r="AS2" s="123"/>
-      <c r="AT2" s="123"/>
-      <c r="AU2" s="123"/>
-      <c r="AV2" s="123"/>
+      <c r="AJ2" s="145"/>
+      <c r="AK2" s="145"/>
+      <c r="AL2" s="145"/>
+      <c r="AM2" s="145"/>
+      <c r="AN2" s="145"/>
+      <c r="AO2" s="145"/>
+      <c r="AP2" s="145"/>
+      <c r="AQ2" s="145"/>
+      <c r="AR2" s="145"/>
+      <c r="AS2" s="145"/>
+      <c r="AT2" s="145"/>
+      <c r="AU2" s="145"/>
+      <c r="AV2" s="145"/>
       <c r="AW2" s="103"/>
       <c r="AX2" s="103"/>
       <c r="AY2" s="103"/>
@@ -2033,17 +2174,17 @@
       <c r="CG2" s="1"/>
       <c r="CH2" s="1"/>
       <c r="CI2" s="1"/>
-      <c r="CJ2" s="1"/>
-      <c r="CK2" s="1"/>
+      <c r="CJ2" s="165"/>
+      <c r="CK2" s="154"/>
       <c r="CL2" s="1"/>
       <c r="CM2" s="1"/>
       <c r="CN2" s="1"/>
       <c r="CO2" s="1"/>
-      <c r="CP2" s="1"/>
+      <c r="CP2" s="154"/>
       <c r="CQ2" s="1"/>
       <c r="CR2" s="1"/>
       <c r="CS2" s="1"/>
-      <c r="CT2" s="1"/>
+      <c r="CT2" s="165"/>
       <c r="CU2" s="1"/>
       <c r="CV2" s="1"/>
       <c r="CW2" s="1"/>
@@ -2154,17 +2295,17 @@
       <c r="CG3" s="3"/>
       <c r="CH3" s="3"/>
       <c r="CI3" s="3"/>
-      <c r="CJ3" s="3"/>
-      <c r="CK3" s="3"/>
+      <c r="CJ3" s="166"/>
+      <c r="CK3" s="155"/>
       <c r="CL3" s="3"/>
       <c r="CM3" s="3"/>
       <c r="CN3" s="3"/>
       <c r="CO3" s="3"/>
-      <c r="CP3" s="3"/>
+      <c r="CP3" s="155"/>
       <c r="CQ3" s="3"/>
       <c r="CR3" s="3"/>
       <c r="CS3" s="3"/>
-      <c r="CT3" s="3"/>
+      <c r="CT3" s="166"/>
       <c r="CU3" s="3"/>
       <c r="CV3" s="3"/>
       <c r="CW3" s="3"/>
@@ -2193,57 +2334,57 @@
       <c r="C4" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="136" t="s">
+      <c r="D4" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="127"/>
-      <c r="F4" s="127"/>
-      <c r="G4" s="127"/>
-      <c r="H4" s="128"/>
-      <c r="I4" s="126" t="s">
+      <c r="E4" s="128"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="146" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="127"/>
-      <c r="K4" s="127"/>
-      <c r="L4" s="127"/>
-      <c r="M4" s="127"/>
-      <c r="N4" s="127"/>
-      <c r="O4" s="127"/>
-      <c r="P4" s="127"/>
-      <c r="Q4" s="128"/>
-      <c r="R4" s="130" t="s">
+      <c r="J4" s="128"/>
+      <c r="K4" s="128"/>
+      <c r="L4" s="128"/>
+      <c r="M4" s="128"/>
+      <c r="N4" s="128"/>
+      <c r="O4" s="128"/>
+      <c r="P4" s="128"/>
+      <c r="Q4" s="129"/>
+      <c r="R4" s="148" t="s">
         <v>5</v>
       </c>
-      <c r="S4" s="127"/>
-      <c r="T4" s="127"/>
-      <c r="U4" s="127"/>
-      <c r="V4" s="127"/>
-      <c r="W4" s="127"/>
-      <c r="X4" s="127"/>
-      <c r="Y4" s="127"/>
-      <c r="Z4" s="127"/>
-      <c r="AA4" s="127"/>
-      <c r="AB4" s="127"/>
-      <c r="AC4" s="127"/>
-      <c r="AD4" s="127"/>
-      <c r="AE4" s="127"/>
-      <c r="AF4" s="127"/>
-      <c r="AG4" s="127"/>
-      <c r="AH4" s="127"/>
-      <c r="AI4" s="127"/>
-      <c r="AJ4" s="127"/>
-      <c r="AK4" s="127"/>
-      <c r="AL4" s="127"/>
-      <c r="AM4" s="127"/>
-      <c r="AN4" s="127"/>
-      <c r="AO4" s="127"/>
-      <c r="AP4" s="127"/>
-      <c r="AQ4" s="127"/>
-      <c r="AR4" s="127"/>
-      <c r="AS4" s="127"/>
-      <c r="AT4" s="127"/>
-      <c r="AU4" s="127"/>
-      <c r="AV4" s="128"/>
+      <c r="S4" s="128"/>
+      <c r="T4" s="128"/>
+      <c r="U4" s="128"/>
+      <c r="V4" s="128"/>
+      <c r="W4" s="128"/>
+      <c r="X4" s="128"/>
+      <c r="Y4" s="128"/>
+      <c r="Z4" s="128"/>
+      <c r="AA4" s="128"/>
+      <c r="AB4" s="128"/>
+      <c r="AC4" s="128"/>
+      <c r="AD4" s="128"/>
+      <c r="AE4" s="128"/>
+      <c r="AF4" s="128"/>
+      <c r="AG4" s="128"/>
+      <c r="AH4" s="128"/>
+      <c r="AI4" s="128"/>
+      <c r="AJ4" s="128"/>
+      <c r="AK4" s="128"/>
+      <c r="AL4" s="128"/>
+      <c r="AM4" s="128"/>
+      <c r="AN4" s="128"/>
+      <c r="AO4" s="128"/>
+      <c r="AP4" s="128"/>
+      <c r="AQ4" s="128"/>
+      <c r="AR4" s="128"/>
+      <c r="AS4" s="128"/>
+      <c r="AT4" s="128"/>
+      <c r="AU4" s="128"/>
+      <c r="AV4" s="129"/>
       <c r="AW4" s="111"/>
       <c r="AX4" s="111"/>
       <c r="AY4" s="111"/>
@@ -2283,17 +2424,17 @@
       <c r="CG4" s="3"/>
       <c r="CH4" s="3"/>
       <c r="CI4" s="3"/>
-      <c r="CJ4" s="3"/>
-      <c r="CK4" s="3"/>
+      <c r="CJ4" s="166"/>
+      <c r="CK4" s="155"/>
       <c r="CL4" s="3"/>
       <c r="CM4" s="3"/>
       <c r="CN4" s="3"/>
       <c r="CO4" s="3"/>
-      <c r="CP4" s="3"/>
+      <c r="CP4" s="155"/>
       <c r="CQ4" s="3"/>
       <c r="CR4" s="3"/>
       <c r="CS4" s="3"/>
-      <c r="CT4" s="3"/>
+      <c r="CT4" s="166"/>
       <c r="CU4" s="3"/>
       <c r="CV4" s="3"/>
       <c r="CW4" s="3"/>
@@ -2322,57 +2463,57 @@
       <c r="C5" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="136" t="s">
+      <c r="D5" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="127"/>
-      <c r="F5" s="127"/>
-      <c r="G5" s="127"/>
-      <c r="H5" s="128"/>
-      <c r="I5" s="126" t="s">
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="129"/>
+      <c r="I5" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="127"/>
-      <c r="K5" s="127"/>
-      <c r="L5" s="127"/>
-      <c r="M5" s="127"/>
-      <c r="N5" s="127"/>
-      <c r="O5" s="127"/>
-      <c r="P5" s="127"/>
-      <c r="Q5" s="128"/>
-      <c r="R5" s="129">
+      <c r="J5" s="128"/>
+      <c r="K5" s="128"/>
+      <c r="L5" s="128"/>
+      <c r="M5" s="128"/>
+      <c r="N5" s="128"/>
+      <c r="O5" s="128"/>
+      <c r="P5" s="128"/>
+      <c r="Q5" s="129"/>
+      <c r="R5" s="147">
         <v>43346</v>
       </c>
-      <c r="S5" s="127"/>
-      <c r="T5" s="127"/>
-      <c r="U5" s="127"/>
-      <c r="V5" s="127"/>
-      <c r="W5" s="127"/>
-      <c r="X5" s="127"/>
-      <c r="Y5" s="127"/>
-      <c r="Z5" s="127"/>
-      <c r="AA5" s="127"/>
-      <c r="AB5" s="127"/>
-      <c r="AC5" s="127"/>
-      <c r="AD5" s="127"/>
-      <c r="AE5" s="127"/>
-      <c r="AF5" s="127"/>
-      <c r="AG5" s="127"/>
-      <c r="AH5" s="127"/>
-      <c r="AI5" s="127"/>
-      <c r="AJ5" s="127"/>
-      <c r="AK5" s="127"/>
-      <c r="AL5" s="127"/>
-      <c r="AM5" s="127"/>
-      <c r="AN5" s="127"/>
-      <c r="AO5" s="127"/>
-      <c r="AP5" s="127"/>
-      <c r="AQ5" s="127"/>
-      <c r="AR5" s="127"/>
-      <c r="AS5" s="127"/>
-      <c r="AT5" s="127"/>
-      <c r="AU5" s="127"/>
-      <c r="AV5" s="128"/>
+      <c r="S5" s="128"/>
+      <c r="T5" s="128"/>
+      <c r="U5" s="128"/>
+      <c r="V5" s="128"/>
+      <c r="W5" s="128"/>
+      <c r="X5" s="128"/>
+      <c r="Y5" s="128"/>
+      <c r="Z5" s="128"/>
+      <c r="AA5" s="128"/>
+      <c r="AB5" s="128"/>
+      <c r="AC5" s="128"/>
+      <c r="AD5" s="128"/>
+      <c r="AE5" s="128"/>
+      <c r="AF5" s="128"/>
+      <c r="AG5" s="128"/>
+      <c r="AH5" s="128"/>
+      <c r="AI5" s="128"/>
+      <c r="AJ5" s="128"/>
+      <c r="AK5" s="128"/>
+      <c r="AL5" s="128"/>
+      <c r="AM5" s="128"/>
+      <c r="AN5" s="128"/>
+      <c r="AO5" s="128"/>
+      <c r="AP5" s="128"/>
+      <c r="AQ5" s="128"/>
+      <c r="AR5" s="128"/>
+      <c r="AS5" s="128"/>
+      <c r="AT5" s="128"/>
+      <c r="AU5" s="128"/>
+      <c r="AV5" s="129"/>
       <c r="AW5" s="111"/>
       <c r="AX5" s="111"/>
       <c r="AY5" s="111"/>
@@ -2412,17 +2553,17 @@
       <c r="CG5" s="3"/>
       <c r="CH5" s="3"/>
       <c r="CI5" s="3"/>
-      <c r="CJ5" s="3"/>
-      <c r="CK5" s="3"/>
+      <c r="CJ5" s="166"/>
+      <c r="CK5" s="155"/>
       <c r="CL5" s="3"/>
       <c r="CM5" s="3"/>
       <c r="CN5" s="3"/>
       <c r="CO5" s="3"/>
-      <c r="CP5" s="3"/>
+      <c r="CP5" s="155"/>
       <c r="CQ5" s="3"/>
       <c r="CR5" s="3"/>
       <c r="CS5" s="3"/>
-      <c r="CT5" s="3"/>
+      <c r="CT5" s="166"/>
       <c r="CU5" s="3"/>
       <c r="CV5" s="3"/>
       <c r="CW5" s="3"/>
@@ -2533,17 +2674,17 @@
       <c r="CG6" s="3"/>
       <c r="CH6" s="3"/>
       <c r="CI6" s="3"/>
-      <c r="CJ6" s="3"/>
-      <c r="CK6" s="3"/>
+      <c r="CJ6" s="166"/>
+      <c r="CK6" s="155"/>
       <c r="CL6" s="3"/>
       <c r="CM6" s="3"/>
       <c r="CN6" s="3"/>
       <c r="CO6" s="3"/>
-      <c r="CP6" s="3"/>
+      <c r="CP6" s="155"/>
       <c r="CQ6" s="3"/>
       <c r="CR6" s="3"/>
       <c r="CS6" s="3"/>
-      <c r="CT6" s="3"/>
+      <c r="CT6" s="166"/>
       <c r="CU6" s="3"/>
       <c r="CV6" s="3"/>
       <c r="CW6" s="3"/>
@@ -2575,55 +2716,55 @@
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
-      <c r="I7" s="131" t="s">
+      <c r="I7" s="149" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="132"/>
-      <c r="K7" s="132"/>
-      <c r="L7" s="132"/>
-      <c r="M7" s="132"/>
-      <c r="N7" s="132"/>
-      <c r="O7" s="132"/>
-      <c r="P7" s="132"/>
-      <c r="Q7" s="132"/>
-      <c r="R7" s="132"/>
-      <c r="S7" s="132"/>
-      <c r="T7" s="132"/>
-      <c r="U7" s="132"/>
-      <c r="V7" s="132"/>
-      <c r="W7" s="132"/>
-      <c r="X7" s="132"/>
-      <c r="Y7" s="132"/>
-      <c r="Z7" s="132"/>
-      <c r="AA7" s="132"/>
-      <c r="AB7" s="133"/>
-      <c r="AC7" s="137" t="s">
+      <c r="J7" s="150"/>
+      <c r="K7" s="150"/>
+      <c r="L7" s="150"/>
+      <c r="M7" s="150"/>
+      <c r="N7" s="150"/>
+      <c r="O7" s="150"/>
+      <c r="P7" s="150"/>
+      <c r="Q7" s="150"/>
+      <c r="R7" s="150"/>
+      <c r="S7" s="150"/>
+      <c r="T7" s="150"/>
+      <c r="U7" s="150"/>
+      <c r="V7" s="150"/>
+      <c r="W7" s="150"/>
+      <c r="X7" s="150"/>
+      <c r="Y7" s="150"/>
+      <c r="Z7" s="150"/>
+      <c r="AA7" s="150"/>
+      <c r="AB7" s="151"/>
+      <c r="AC7" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="AD7" s="138"/>
-      <c r="AE7" s="138"/>
-      <c r="AF7" s="138"/>
-      <c r="AG7" s="138"/>
-      <c r="AH7" s="138"/>
-      <c r="AI7" s="138"/>
-      <c r="AJ7" s="138"/>
-      <c r="AK7" s="138"/>
-      <c r="AL7" s="138"/>
-      <c r="AM7" s="138"/>
-      <c r="AN7" s="138"/>
-      <c r="AO7" s="138"/>
-      <c r="AP7" s="138"/>
-      <c r="AQ7" s="138"/>
-      <c r="AR7" s="138"/>
-      <c r="AS7" s="138"/>
-      <c r="AT7" s="138"/>
-      <c r="AU7" s="138"/>
-      <c r="AV7" s="138"/>
-      <c r="AW7" s="138"/>
-      <c r="AX7" s="138"/>
-      <c r="AY7" s="138"/>
-      <c r="AZ7" s="138"/>
-      <c r="BA7" s="138"/>
+      <c r="AD7" s="139"/>
+      <c r="AE7" s="139"/>
+      <c r="AF7" s="139"/>
+      <c r="AG7" s="139"/>
+      <c r="AH7" s="139"/>
+      <c r="AI7" s="139"/>
+      <c r="AJ7" s="139"/>
+      <c r="AK7" s="139"/>
+      <c r="AL7" s="139"/>
+      <c r="AM7" s="139"/>
+      <c r="AN7" s="139"/>
+      <c r="AO7" s="139"/>
+      <c r="AP7" s="139"/>
+      <c r="AQ7" s="139"/>
+      <c r="AR7" s="139"/>
+      <c r="AS7" s="139"/>
+      <c r="AT7" s="139"/>
+      <c r="AU7" s="139"/>
+      <c r="AV7" s="139"/>
+      <c r="AW7" s="139"/>
+      <c r="AX7" s="139"/>
+      <c r="AY7" s="139"/>
+      <c r="AZ7" s="139"/>
+      <c r="BA7" s="139"/>
       <c r="BB7" s="142" t="s">
         <v>11</v>
       </c>
@@ -2646,245 +2787,245 @@
       <c r="BS7" s="142"/>
       <c r="BT7" s="142"/>
       <c r="BU7" s="142"/>
-      <c r="BV7" s="140" t="s">
+      <c r="BV7" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="BW7" s="140"/>
-      <c r="BX7" s="140"/>
-      <c r="BY7" s="140"/>
-      <c r="BZ7" s="140"/>
-      <c r="CA7" s="140"/>
-      <c r="CB7" s="140"/>
-      <c r="CC7" s="140"/>
-      <c r="CD7" s="140"/>
-      <c r="CE7" s="140"/>
-      <c r="CF7" s="140"/>
-      <c r="CG7" s="140"/>
-      <c r="CH7" s="140"/>
-      <c r="CI7" s="140"/>
-      <c r="CJ7" s="140"/>
-      <c r="CK7" s="140"/>
-      <c r="CL7" s="140"/>
-      <c r="CM7" s="140"/>
-      <c r="CN7" s="140"/>
-      <c r="CO7" s="140"/>
-      <c r="CP7" s="140"/>
-      <c r="CQ7" s="140"/>
-      <c r="CR7" s="140"/>
-      <c r="CS7" s="140"/>
-      <c r="CT7" s="140"/>
-      <c r="CU7" s="139" t="s">
+      <c r="BW7" s="141"/>
+      <c r="BX7" s="141"/>
+      <c r="BY7" s="141"/>
+      <c r="BZ7" s="141"/>
+      <c r="CA7" s="141"/>
+      <c r="CB7" s="141"/>
+      <c r="CC7" s="141"/>
+      <c r="CD7" s="141"/>
+      <c r="CE7" s="141"/>
+      <c r="CF7" s="141"/>
+      <c r="CG7" s="141"/>
+      <c r="CH7" s="141"/>
+      <c r="CI7" s="141"/>
+      <c r="CJ7" s="141"/>
+      <c r="CK7" s="141"/>
+      <c r="CL7" s="141"/>
+      <c r="CM7" s="141"/>
+      <c r="CN7" s="141"/>
+      <c r="CO7" s="141"/>
+      <c r="CP7" s="141"/>
+      <c r="CQ7" s="141"/>
+      <c r="CR7" s="141"/>
+      <c r="CS7" s="141"/>
+      <c r="CT7" s="141"/>
+      <c r="CU7" s="140" t="s">
         <v>13</v>
       </c>
-      <c r="CV7" s="139"/>
-      <c r="CW7" s="139"/>
-      <c r="CX7" s="139"/>
-      <c r="CY7" s="139"/>
-      <c r="CZ7" s="139"/>
-      <c r="DA7" s="139"/>
-      <c r="DB7" s="139"/>
-      <c r="DC7" s="139"/>
-      <c r="DD7" s="139"/>
-      <c r="DE7" s="139"/>
-      <c r="DF7" s="139"/>
-      <c r="DG7" s="139"/>
-      <c r="DH7" s="139"/>
-      <c r="DI7" s="139"/>
-      <c r="DJ7" s="139"/>
-      <c r="DK7" s="139"/>
-      <c r="DL7" s="139"/>
-      <c r="DM7" s="139"/>
-      <c r="DN7" s="139"/>
+      <c r="CV7" s="140"/>
+      <c r="CW7" s="140"/>
+      <c r="CX7" s="140"/>
+      <c r="CY7" s="140"/>
+      <c r="CZ7" s="140"/>
+      <c r="DA7" s="140"/>
+      <c r="DB7" s="140"/>
+      <c r="DC7" s="140"/>
+      <c r="DD7" s="140"/>
+      <c r="DE7" s="140"/>
+      <c r="DF7" s="140"/>
+      <c r="DG7" s="140"/>
+      <c r="DH7" s="140"/>
+      <c r="DI7" s="140"/>
+      <c r="DJ7" s="140"/>
+      <c r="DK7" s="140"/>
+      <c r="DL7" s="140"/>
+      <c r="DM7" s="140"/>
+      <c r="DN7" s="140"/>
       <c r="DO7" s="7"/>
     </row>
     <row r="8" spans="1:119" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="148" t="s">
+      <c r="B8" s="125" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="124" t="s">
+      <c r="C8" s="134" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="124" t="s">
+      <c r="D8" s="134" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="124" t="s">
+      <c r="E8" s="134" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="124" t="s">
+      <c r="F8" s="134" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="124" t="s">
+      <c r="G8" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="150" t="s">
+      <c r="H8" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="134" t="s">
+      <c r="I8" s="127" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="127"/>
-      <c r="K8" s="127"/>
-      <c r="L8" s="127"/>
-      <c r="M8" s="128"/>
-      <c r="N8" s="134" t="s">
+      <c r="J8" s="128"/>
+      <c r="K8" s="128"/>
+      <c r="L8" s="128"/>
+      <c r="M8" s="129"/>
+      <c r="N8" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="127"/>
-      <c r="P8" s="127"/>
-      <c r="Q8" s="127"/>
-      <c r="R8" s="128"/>
-      <c r="S8" s="134" t="s">
+      <c r="O8" s="128"/>
+      <c r="P8" s="128"/>
+      <c r="Q8" s="128"/>
+      <c r="R8" s="129"/>
+      <c r="S8" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="T8" s="127"/>
-      <c r="U8" s="127"/>
-      <c r="V8" s="127"/>
-      <c r="W8" s="128"/>
-      <c r="X8" s="134" t="s">
+      <c r="T8" s="128"/>
+      <c r="U8" s="128"/>
+      <c r="V8" s="128"/>
+      <c r="W8" s="129"/>
+      <c r="X8" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="Y8" s="127"/>
-      <c r="Z8" s="127"/>
-      <c r="AA8" s="127"/>
-      <c r="AB8" s="128"/>
-      <c r="AC8" s="135" t="s">
+      <c r="Y8" s="128"/>
+      <c r="Z8" s="128"/>
+      <c r="AA8" s="128"/>
+      <c r="AB8" s="129"/>
+      <c r="AC8" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="AD8" s="127"/>
-      <c r="AE8" s="127"/>
-      <c r="AF8" s="127"/>
-      <c r="AG8" s="128"/>
-      <c r="AH8" s="135" t="s">
+      <c r="AD8" s="128"/>
+      <c r="AE8" s="128"/>
+      <c r="AF8" s="128"/>
+      <c r="AG8" s="129"/>
+      <c r="AH8" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="AI8" s="127"/>
-      <c r="AJ8" s="127"/>
-      <c r="AK8" s="127"/>
-      <c r="AL8" s="128"/>
-      <c r="AM8" s="135" t="s">
+      <c r="AI8" s="128"/>
+      <c r="AJ8" s="128"/>
+      <c r="AK8" s="128"/>
+      <c r="AL8" s="129"/>
+      <c r="AM8" s="131" t="s">
         <v>27</v>
       </c>
-      <c r="AN8" s="127"/>
-      <c r="AO8" s="127"/>
-      <c r="AP8" s="127"/>
-      <c r="AQ8" s="128"/>
-      <c r="AR8" s="135" t="s">
+      <c r="AN8" s="128"/>
+      <c r="AO8" s="128"/>
+      <c r="AP8" s="128"/>
+      <c r="AQ8" s="129"/>
+      <c r="AR8" s="131" t="s">
         <v>28</v>
       </c>
-      <c r="AS8" s="127"/>
-      <c r="AT8" s="127"/>
-      <c r="AU8" s="127"/>
-      <c r="AV8" s="128"/>
-      <c r="AW8" s="135" t="s">
+      <c r="AS8" s="128"/>
+      <c r="AT8" s="128"/>
+      <c r="AU8" s="128"/>
+      <c r="AV8" s="129"/>
+      <c r="AW8" s="131" t="s">
         <v>29</v>
       </c>
-      <c r="AX8" s="127"/>
-      <c r="AY8" s="127"/>
-      <c r="AZ8" s="127"/>
-      <c r="BA8" s="128"/>
-      <c r="BB8" s="141" t="s">
+      <c r="AX8" s="128"/>
+      <c r="AY8" s="128"/>
+      <c r="AZ8" s="128"/>
+      <c r="BA8" s="129"/>
+      <c r="BB8" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="BC8" s="127"/>
-      <c r="BD8" s="127"/>
-      <c r="BE8" s="127"/>
-      <c r="BF8" s="128"/>
-      <c r="BG8" s="141" t="s">
+      <c r="BC8" s="128"/>
+      <c r="BD8" s="128"/>
+      <c r="BE8" s="128"/>
+      <c r="BF8" s="129"/>
+      <c r="BG8" s="130" t="s">
         <v>31</v>
       </c>
-      <c r="BH8" s="127"/>
-      <c r="BI8" s="127"/>
-      <c r="BJ8" s="127"/>
-      <c r="BK8" s="128"/>
-      <c r="BL8" s="141" t="s">
+      <c r="BH8" s="128"/>
+      <c r="BI8" s="128"/>
+      <c r="BJ8" s="128"/>
+      <c r="BK8" s="129"/>
+      <c r="BL8" s="130" t="s">
         <v>32</v>
       </c>
-      <c r="BM8" s="127"/>
-      <c r="BN8" s="127"/>
-      <c r="BO8" s="127"/>
-      <c r="BP8" s="128"/>
-      <c r="BQ8" s="141" t="s">
+      <c r="BM8" s="128"/>
+      <c r="BN8" s="128"/>
+      <c r="BO8" s="128"/>
+      <c r="BP8" s="129"/>
+      <c r="BQ8" s="130" t="s">
         <v>33</v>
       </c>
-      <c r="BR8" s="127"/>
-      <c r="BS8" s="127"/>
-      <c r="BT8" s="127"/>
-      <c r="BU8" s="128"/>
-      <c r="BV8" s="143" t="s">
+      <c r="BR8" s="128"/>
+      <c r="BS8" s="128"/>
+      <c r="BT8" s="128"/>
+      <c r="BU8" s="129"/>
+      <c r="BV8" s="136" t="s">
         <v>34</v>
       </c>
-      <c r="BW8" s="127"/>
-      <c r="BX8" s="127"/>
-      <c r="BY8" s="127"/>
-      <c r="BZ8" s="128"/>
-      <c r="CA8" s="143" t="s">
+      <c r="BW8" s="128"/>
+      <c r="BX8" s="128"/>
+      <c r="BY8" s="128"/>
+      <c r="BZ8" s="129"/>
+      <c r="CA8" s="136" t="s">
         <v>35</v>
       </c>
-      <c r="CB8" s="127"/>
-      <c r="CC8" s="127"/>
-      <c r="CD8" s="127"/>
-      <c r="CE8" s="128"/>
-      <c r="CF8" s="143" t="s">
+      <c r="CB8" s="128"/>
+      <c r="CC8" s="128"/>
+      <c r="CD8" s="128"/>
+      <c r="CE8" s="129"/>
+      <c r="CF8" s="136" t="s">
         <v>36</v>
       </c>
-      <c r="CG8" s="127"/>
-      <c r="CH8" s="127"/>
-      <c r="CI8" s="127"/>
-      <c r="CJ8" s="128"/>
-      <c r="CK8" s="143" t="s">
+      <c r="CG8" s="128"/>
+      <c r="CH8" s="128"/>
+      <c r="CI8" s="128"/>
+      <c r="CJ8" s="129"/>
+      <c r="CK8" s="136" t="s">
         <v>37</v>
       </c>
-      <c r="CL8" s="127"/>
-      <c r="CM8" s="127"/>
-      <c r="CN8" s="127"/>
-      <c r="CO8" s="128"/>
-      <c r="CP8" s="143" t="s">
+      <c r="CL8" s="128"/>
+      <c r="CM8" s="128"/>
+      <c r="CN8" s="128"/>
+      <c r="CO8" s="129"/>
+      <c r="CP8" s="136" t="s">
         <v>38</v>
       </c>
-      <c r="CQ8" s="127"/>
-      <c r="CR8" s="127"/>
-      <c r="CS8" s="127"/>
-      <c r="CT8" s="128"/>
-      <c r="CU8" s="144" t="s">
+      <c r="CQ8" s="128"/>
+      <c r="CR8" s="128"/>
+      <c r="CS8" s="128"/>
+      <c r="CT8" s="129"/>
+      <c r="CU8" s="143" t="s">
         <v>39</v>
       </c>
-      <c r="CV8" s="127"/>
-      <c r="CW8" s="127"/>
-      <c r="CX8" s="127"/>
-      <c r="CY8" s="128"/>
-      <c r="CZ8" s="144" t="s">
+      <c r="CV8" s="128"/>
+      <c r="CW8" s="128"/>
+      <c r="CX8" s="128"/>
+      <c r="CY8" s="129"/>
+      <c r="CZ8" s="143" t="s">
         <v>40</v>
       </c>
-      <c r="DA8" s="127"/>
-      <c r="DB8" s="127"/>
-      <c r="DC8" s="127"/>
-      <c r="DD8" s="128"/>
-      <c r="DE8" s="144" t="s">
+      <c r="DA8" s="128"/>
+      <c r="DB8" s="128"/>
+      <c r="DC8" s="128"/>
+      <c r="DD8" s="129"/>
+      <c r="DE8" s="143" t="s">
         <v>41</v>
       </c>
-      <c r="DF8" s="127"/>
-      <c r="DG8" s="127"/>
-      <c r="DH8" s="127"/>
-      <c r="DI8" s="128"/>
-      <c r="DJ8" s="144" t="s">
+      <c r="DF8" s="128"/>
+      <c r="DG8" s="128"/>
+      <c r="DH8" s="128"/>
+      <c r="DI8" s="129"/>
+      <c r="DJ8" s="143" t="s">
         <v>42</v>
       </c>
-      <c r="DK8" s="127"/>
-      <c r="DL8" s="127"/>
-      <c r="DM8" s="127"/>
-      <c r="DN8" s="128"/>
+      <c r="DK8" s="128"/>
+      <c r="DL8" s="128"/>
+      <c r="DM8" s="128"/>
+      <c r="DN8" s="129"/>
       <c r="DO8" s="8"/>
     </row>
     <row r="9" spans="1:119" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="149"/>
-      <c r="C9" s="125"/>
-      <c r="D9" s="125"/>
-      <c r="E9" s="125"/>
-      <c r="F9" s="125"/>
-      <c r="G9" s="125"/>
-      <c r="H9" s="151"/>
+      <c r="B9" s="126"/>
+      <c r="C9" s="135"/>
+      <c r="D9" s="135"/>
+      <c r="E9" s="135"/>
+      <c r="F9" s="135"/>
+      <c r="G9" s="135"/>
+      <c r="H9" s="133"/>
       <c r="I9" s="20" t="s">
         <v>43</v>
       </c>
@@ -3122,10 +3263,10 @@
       <c r="CI9" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="CJ9" s="24" t="s">
+      <c r="CJ9" s="167" t="s">
         <v>47</v>
       </c>
-      <c r="CK9" s="24" t="s">
+      <c r="CK9" s="156" t="s">
         <v>43</v>
       </c>
       <c r="CL9" s="24" t="s">
@@ -3140,7 +3281,7 @@
       <c r="CO9" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="CP9" s="24" t="s">
+      <c r="CP9" s="156" t="s">
         <v>43</v>
       </c>
       <c r="CQ9" s="25" t="s">
@@ -3152,7 +3293,7 @@
       <c r="CS9" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="CT9" s="25" t="s">
+      <c r="CT9" s="177" t="s">
         <v>47</v>
       </c>
       <c r="CU9" s="25" t="s">
@@ -3477,10 +3618,10 @@
       <c r="CI10" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="CJ10" s="38" t="s">
+      <c r="CJ10" s="168" t="s">
         <v>62</v>
       </c>
-      <c r="CK10" s="37" t="s">
+      <c r="CK10" s="152" t="s">
         <v>63</v>
       </c>
       <c r="CL10" s="37" t="s">
@@ -3495,7 +3636,7 @@
       <c r="CO10" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="CP10" s="38" t="s">
+      <c r="CP10" s="153" t="s">
         <v>78</v>
       </c>
       <c r="CQ10" s="39" t="s">
@@ -3507,7 +3648,7 @@
       <c r="CS10" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="CT10" s="39" t="s">
+      <c r="CT10" s="178" t="s">
         <v>49</v>
       </c>
       <c r="CU10" s="40" t="s">
@@ -3664,17 +3805,17 @@
       <c r="CG11" s="45"/>
       <c r="CH11" s="45"/>
       <c r="CI11" s="45"/>
-      <c r="CJ11" s="45"/>
-      <c r="CK11" s="45"/>
+      <c r="CJ11" s="169"/>
+      <c r="CK11" s="157"/>
       <c r="CL11" s="45"/>
       <c r="CM11" s="45"/>
       <c r="CN11" s="45"/>
       <c r="CO11" s="45"/>
-      <c r="CP11" s="45"/>
+      <c r="CP11" s="157"/>
       <c r="CQ11" s="45"/>
       <c r="CR11" s="45"/>
       <c r="CS11" s="45"/>
-      <c r="CT11" s="45"/>
+      <c r="CT11" s="169"/>
       <c r="CU11" s="45"/>
       <c r="CV11" s="45"/>
       <c r="CW11" s="45"/>
@@ -3800,17 +3941,17 @@
       <c r="CG12" s="62"/>
       <c r="CH12" s="24"/>
       <c r="CI12" s="62"/>
-      <c r="CJ12" s="62"/>
-      <c r="CK12" s="59"/>
+      <c r="CJ12" s="170"/>
+      <c r="CK12" s="163"/>
       <c r="CL12" s="59"/>
       <c r="CM12" s="24"/>
       <c r="CN12" s="59"/>
       <c r="CO12" s="59"/>
-      <c r="CP12" s="62"/>
+      <c r="CP12" s="158"/>
       <c r="CQ12" s="63"/>
       <c r="CR12" s="64"/>
       <c r="CS12" s="63"/>
-      <c r="CT12" s="63"/>
+      <c r="CT12" s="179"/>
       <c r="CU12" s="59"/>
       <c r="CV12" s="59"/>
       <c r="CW12" s="64"/>
@@ -3936,17 +4077,17 @@
       <c r="CG13" s="24"/>
       <c r="CH13" s="24"/>
       <c r="CI13" s="24"/>
-      <c r="CJ13" s="24"/>
-      <c r="CK13" s="24"/>
+      <c r="CJ13" s="167"/>
+      <c r="CK13" s="156"/>
       <c r="CL13" s="24"/>
       <c r="CM13" s="24"/>
       <c r="CN13" s="24"/>
       <c r="CO13" s="24"/>
-      <c r="CP13" s="24"/>
+      <c r="CP13" s="156"/>
       <c r="CQ13" s="64"/>
       <c r="CR13" s="64"/>
       <c r="CS13" s="64"/>
-      <c r="CT13" s="64"/>
+      <c r="CT13" s="180"/>
       <c r="CU13" s="64"/>
       <c r="CV13" s="64"/>
       <c r="CW13" s="64"/>
@@ -4072,17 +4213,17 @@
       <c r="CG14" s="62"/>
       <c r="CH14" s="62"/>
       <c r="CI14" s="62"/>
-      <c r="CJ14" s="62"/>
-      <c r="CK14" s="24"/>
+      <c r="CJ14" s="170"/>
+      <c r="CK14" s="156"/>
       <c r="CL14" s="59"/>
       <c r="CM14" s="59"/>
       <c r="CN14" s="59"/>
       <c r="CO14" s="59"/>
-      <c r="CP14" s="24"/>
+      <c r="CP14" s="156"/>
       <c r="CQ14" s="63"/>
       <c r="CR14" s="63"/>
       <c r="CS14" s="63"/>
-      <c r="CT14" s="63"/>
+      <c r="CT14" s="179"/>
       <c r="CU14" s="64"/>
       <c r="CV14" s="59"/>
       <c r="CW14" s="59"/>
@@ -4208,17 +4349,17 @@
       <c r="CG15" s="62"/>
       <c r="CH15" s="62"/>
       <c r="CI15" s="62"/>
-      <c r="CJ15" s="62"/>
-      <c r="CK15" s="59"/>
+      <c r="CJ15" s="170"/>
+      <c r="CK15" s="163"/>
       <c r="CL15" s="59"/>
       <c r="CM15" s="59"/>
       <c r="CN15" s="59"/>
       <c r="CO15" s="59"/>
-      <c r="CP15" s="62"/>
+      <c r="CP15" s="158"/>
       <c r="CQ15" s="63"/>
       <c r="CR15" s="63"/>
       <c r="CS15" s="63"/>
-      <c r="CT15" s="63"/>
+      <c r="CT15" s="179"/>
       <c r="CU15" s="59"/>
       <c r="CV15" s="59"/>
       <c r="CW15" s="59"/>
@@ -4344,17 +4485,17 @@
       <c r="CG16" s="24"/>
       <c r="CH16" s="24"/>
       <c r="CI16" s="24"/>
-      <c r="CJ16" s="24"/>
-      <c r="CK16" s="24"/>
+      <c r="CJ16" s="167"/>
+      <c r="CK16" s="156"/>
       <c r="CL16" s="24"/>
       <c r="CM16" s="24"/>
       <c r="CN16" s="24"/>
       <c r="CO16" s="24"/>
-      <c r="CP16" s="24"/>
+      <c r="CP16" s="156"/>
       <c r="CQ16" s="64"/>
       <c r="CR16" s="64"/>
       <c r="CS16" s="64"/>
-      <c r="CT16" s="64"/>
+      <c r="CT16" s="180"/>
       <c r="CU16" s="64"/>
       <c r="CV16" s="64"/>
       <c r="CW16" s="64"/>
@@ -4480,17 +4621,17 @@
       <c r="CG17" s="24"/>
       <c r="CH17" s="24"/>
       <c r="CI17" s="24"/>
-      <c r="CJ17" s="24"/>
-      <c r="CK17" s="24"/>
+      <c r="CJ17" s="167"/>
+      <c r="CK17" s="156"/>
       <c r="CL17" s="24"/>
       <c r="CM17" s="24"/>
       <c r="CN17" s="24"/>
       <c r="CO17" s="24"/>
-      <c r="CP17" s="24"/>
+      <c r="CP17" s="156"/>
       <c r="CQ17" s="64"/>
       <c r="CR17" s="64"/>
       <c r="CS17" s="64"/>
-      <c r="CT17" s="64"/>
+      <c r="CT17" s="180"/>
       <c r="CU17" s="64"/>
       <c r="CV17" s="64"/>
       <c r="CW17" s="64"/>
@@ -4615,17 +4756,17 @@
       <c r="CG18" s="62"/>
       <c r="CH18" s="62"/>
       <c r="CI18" s="62"/>
-      <c r="CJ18" s="62"/>
-      <c r="CK18" s="59"/>
+      <c r="CJ18" s="170"/>
+      <c r="CK18" s="163"/>
       <c r="CL18" s="59"/>
       <c r="CM18" s="59"/>
       <c r="CN18" s="59"/>
       <c r="CO18" s="59"/>
-      <c r="CP18" s="62"/>
+      <c r="CP18" s="158"/>
       <c r="CQ18" s="63"/>
       <c r="CR18" s="63"/>
       <c r="CS18" s="63"/>
-      <c r="CT18" s="63"/>
+      <c r="CT18" s="179"/>
       <c r="CU18" s="70"/>
       <c r="CV18" s="71"/>
       <c r="CW18" s="64"/>
@@ -4751,17 +4892,17 @@
       <c r="CG19" s="62"/>
       <c r="CH19" s="62"/>
       <c r="CI19" s="62"/>
-      <c r="CJ19" s="62"/>
-      <c r="CK19" s="59"/>
+      <c r="CJ19" s="170"/>
+      <c r="CK19" s="163"/>
       <c r="CL19" s="59"/>
       <c r="CM19" s="59"/>
       <c r="CN19" s="59"/>
       <c r="CO19" s="59"/>
-      <c r="CP19" s="62"/>
+      <c r="CP19" s="158"/>
       <c r="CQ19" s="63"/>
       <c r="CR19" s="63"/>
       <c r="CS19" s="63"/>
-      <c r="CT19" s="63"/>
+      <c r="CT19" s="179"/>
       <c r="CU19" s="70"/>
       <c r="CV19" s="71"/>
       <c r="CW19" s="71"/>
@@ -4887,17 +5028,17 @@
       <c r="CG20" s="62"/>
       <c r="CH20" s="62"/>
       <c r="CI20" s="62"/>
-      <c r="CJ20" s="62"/>
-      <c r="CK20" s="24"/>
+      <c r="CJ20" s="170"/>
+      <c r="CK20" s="156"/>
       <c r="CL20" s="59"/>
       <c r="CM20" s="59"/>
       <c r="CN20" s="59"/>
       <c r="CO20" s="59"/>
-      <c r="CP20" s="62"/>
+      <c r="CP20" s="158"/>
       <c r="CQ20" s="63"/>
       <c r="CR20" s="63"/>
       <c r="CS20" s="63"/>
-      <c r="CT20" s="63"/>
+      <c r="CT20" s="179"/>
       <c r="CU20" s="64"/>
       <c r="CV20" s="71"/>
       <c r="CW20" s="71"/>
@@ -5012,17 +5153,17 @@
       <c r="CG21" s="74"/>
       <c r="CH21" s="74"/>
       <c r="CI21" s="74"/>
-      <c r="CJ21" s="74"/>
-      <c r="CK21" s="74"/>
+      <c r="CJ21" s="171"/>
+      <c r="CK21" s="159"/>
       <c r="CL21" s="74"/>
       <c r="CM21" s="74"/>
       <c r="CN21" s="74"/>
       <c r="CO21" s="74"/>
-      <c r="CP21" s="74"/>
+      <c r="CP21" s="159"/>
       <c r="CQ21" s="74"/>
       <c r="CR21" s="74"/>
       <c r="CS21" s="74"/>
-      <c r="CT21" s="74"/>
+      <c r="CT21" s="171"/>
       <c r="CU21" s="74"/>
       <c r="CV21" s="74"/>
       <c r="CW21" s="74"/>
@@ -5148,17 +5289,17 @@
       <c r="CG22" s="77"/>
       <c r="CH22" s="77"/>
       <c r="CI22" s="77"/>
-      <c r="CJ22" s="77"/>
-      <c r="CK22" s="59"/>
+      <c r="CJ22" s="172"/>
+      <c r="CK22" s="163"/>
       <c r="CL22" s="59"/>
       <c r="CM22" s="59"/>
       <c r="CN22" s="59"/>
       <c r="CO22" s="59"/>
-      <c r="CP22" s="77"/>
+      <c r="CP22" s="160"/>
       <c r="CQ22" s="63"/>
       <c r="CR22" s="63"/>
       <c r="CS22" s="63"/>
-      <c r="CT22" s="63"/>
+      <c r="CT22" s="179"/>
       <c r="CU22" s="59"/>
       <c r="CV22" s="59"/>
       <c r="CW22" s="59"/>
@@ -5284,17 +5425,17 @@
       <c r="CG23" s="79"/>
       <c r="CH23" s="79"/>
       <c r="CI23" s="79"/>
-      <c r="CJ23" s="79"/>
-      <c r="CK23" s="59"/>
+      <c r="CJ23" s="173"/>
+      <c r="CK23" s="163"/>
       <c r="CL23" s="59"/>
       <c r="CM23" s="59"/>
       <c r="CN23" s="59"/>
       <c r="CO23" s="59"/>
-      <c r="CP23" s="79"/>
+      <c r="CP23" s="161"/>
       <c r="CQ23" s="63"/>
       <c r="CR23" s="63"/>
       <c r="CS23" s="63"/>
-      <c r="CT23" s="63"/>
+      <c r="CT23" s="179"/>
       <c r="CU23" s="59"/>
       <c r="CV23" s="59"/>
       <c r="CW23" s="59"/>
@@ -5420,17 +5561,17 @@
       <c r="CG24" s="79"/>
       <c r="CH24" s="79"/>
       <c r="CI24" s="79"/>
-      <c r="CJ24" s="79"/>
-      <c r="CK24" s="59"/>
+      <c r="CJ24" s="173"/>
+      <c r="CK24" s="163"/>
       <c r="CL24" s="59"/>
       <c r="CM24" s="59"/>
       <c r="CN24" s="59"/>
       <c r="CO24" s="59"/>
-      <c r="CP24" s="79"/>
+      <c r="CP24" s="161"/>
       <c r="CQ24" s="63"/>
       <c r="CR24" s="63"/>
       <c r="CS24" s="63"/>
-      <c r="CT24" s="63"/>
+      <c r="CT24" s="179"/>
       <c r="CU24" s="59"/>
       <c r="CV24" s="59"/>
       <c r="CW24" s="59"/>
@@ -5556,17 +5697,17 @@
       <c r="CG25" s="79"/>
       <c r="CH25" s="79"/>
       <c r="CI25" s="79"/>
-      <c r="CJ25" s="79"/>
-      <c r="CK25" s="59"/>
+      <c r="CJ25" s="173"/>
+      <c r="CK25" s="163"/>
       <c r="CL25" s="59"/>
       <c r="CM25" s="59"/>
       <c r="CN25" s="59"/>
       <c r="CO25" s="59"/>
-      <c r="CP25" s="79"/>
+      <c r="CP25" s="161"/>
       <c r="CQ25" s="63"/>
       <c r="CR25" s="63"/>
       <c r="CS25" s="63"/>
-      <c r="CT25" s="63"/>
+      <c r="CT25" s="179"/>
       <c r="CU25" s="59"/>
       <c r="CV25" s="59"/>
       <c r="CW25" s="59"/>
@@ -5685,17 +5826,17 @@
       <c r="CG26" s="79"/>
       <c r="CH26" s="79"/>
       <c r="CI26" s="79"/>
-      <c r="CJ26" s="79"/>
-      <c r="CK26" s="59"/>
+      <c r="CJ26" s="173"/>
+      <c r="CK26" s="163"/>
       <c r="CL26" s="59"/>
       <c r="CM26" s="59"/>
       <c r="CN26" s="59"/>
       <c r="CO26" s="59"/>
-      <c r="CP26" s="79"/>
+      <c r="CP26" s="161"/>
       <c r="CQ26" s="63"/>
       <c r="CR26" s="63"/>
       <c r="CS26" s="63"/>
-      <c r="CT26" s="63"/>
+      <c r="CT26" s="179"/>
       <c r="CU26" s="59"/>
       <c r="CV26" s="59"/>
       <c r="CW26" s="59"/>
@@ -5814,17 +5955,17 @@
       <c r="CG27" s="79"/>
       <c r="CH27" s="79"/>
       <c r="CI27" s="79"/>
-      <c r="CJ27" s="79"/>
-      <c r="CK27" s="59"/>
+      <c r="CJ27" s="173"/>
+      <c r="CK27" s="163"/>
       <c r="CL27" s="59"/>
       <c r="CM27" s="59"/>
       <c r="CN27" s="59"/>
       <c r="CO27" s="59"/>
-      <c r="CP27" s="79"/>
+      <c r="CP27" s="161"/>
       <c r="CQ27" s="63"/>
       <c r="CR27" s="63"/>
       <c r="CS27" s="63"/>
-      <c r="CT27" s="63"/>
+      <c r="CT27" s="179"/>
       <c r="CU27" s="59"/>
       <c r="CV27" s="59"/>
       <c r="CW27" s="59"/>
@@ -5943,17 +6084,17 @@
       <c r="CG28" s="79"/>
       <c r="CH28" s="79"/>
       <c r="CI28" s="79"/>
-      <c r="CJ28" s="79"/>
-      <c r="CK28" s="59"/>
+      <c r="CJ28" s="173"/>
+      <c r="CK28" s="163"/>
       <c r="CL28" s="59"/>
       <c r="CM28" s="59"/>
       <c r="CN28" s="59"/>
       <c r="CO28" s="59"/>
-      <c r="CP28" s="79"/>
+      <c r="CP28" s="161"/>
       <c r="CQ28" s="63"/>
       <c r="CR28" s="63"/>
       <c r="CS28" s="63"/>
-      <c r="CT28" s="63"/>
+      <c r="CT28" s="179"/>
       <c r="CU28" s="59"/>
       <c r="CV28" s="59"/>
       <c r="CW28" s="59"/>
@@ -6072,17 +6213,17 @@
       <c r="CG29" s="79"/>
       <c r="CH29" s="79"/>
       <c r="CI29" s="79"/>
-      <c r="CJ29" s="79"/>
-      <c r="CK29" s="59"/>
+      <c r="CJ29" s="173"/>
+      <c r="CK29" s="163"/>
       <c r="CL29" s="59"/>
       <c r="CM29" s="59"/>
       <c r="CN29" s="59"/>
       <c r="CO29" s="59"/>
-      <c r="CP29" s="79"/>
+      <c r="CP29" s="161"/>
       <c r="CQ29" s="63"/>
       <c r="CR29" s="63"/>
       <c r="CS29" s="63"/>
-      <c r="CT29" s="63"/>
+      <c r="CT29" s="179"/>
       <c r="CU29" s="59"/>
       <c r="CV29" s="59"/>
       <c r="CW29" s="59"/>
@@ -6201,17 +6342,17 @@
       <c r="CG30" s="79"/>
       <c r="CH30" s="79"/>
       <c r="CI30" s="79"/>
-      <c r="CJ30" s="79"/>
-      <c r="CK30" s="59"/>
+      <c r="CJ30" s="173"/>
+      <c r="CK30" s="163"/>
       <c r="CL30" s="59"/>
       <c r="CM30" s="59"/>
       <c r="CN30" s="59"/>
       <c r="CO30" s="59"/>
-      <c r="CP30" s="79"/>
+      <c r="CP30" s="161"/>
       <c r="CQ30" s="63"/>
       <c r="CR30" s="63"/>
       <c r="CS30" s="63"/>
-      <c r="CT30" s="63"/>
+      <c r="CT30" s="179"/>
       <c r="CU30" s="59"/>
       <c r="CV30" s="59"/>
       <c r="CW30" s="59"/>
@@ -6330,17 +6471,17 @@
       <c r="CG31" s="79"/>
       <c r="CH31" s="79"/>
       <c r="CI31" s="79"/>
-      <c r="CJ31" s="79"/>
-      <c r="CK31" s="59"/>
+      <c r="CJ31" s="173"/>
+      <c r="CK31" s="163"/>
       <c r="CL31" s="59"/>
       <c r="CM31" s="59"/>
       <c r="CN31" s="59"/>
       <c r="CO31" s="59"/>
-      <c r="CP31" s="79"/>
+      <c r="CP31" s="161"/>
       <c r="CQ31" s="63"/>
       <c r="CR31" s="63"/>
       <c r="CS31" s="63"/>
-      <c r="CT31" s="63"/>
+      <c r="CT31" s="179"/>
       <c r="CU31" s="59"/>
       <c r="CV31" s="59"/>
       <c r="CW31" s="59"/>
@@ -6466,17 +6607,17 @@
       <c r="CG32" s="79"/>
       <c r="CH32" s="79"/>
       <c r="CI32" s="79"/>
-      <c r="CJ32" s="79"/>
-      <c r="CK32" s="59"/>
+      <c r="CJ32" s="173"/>
+      <c r="CK32" s="163"/>
       <c r="CL32" s="59"/>
       <c r="CM32" s="59"/>
       <c r="CN32" s="59"/>
       <c r="CO32" s="59"/>
-      <c r="CP32" s="79"/>
+      <c r="CP32" s="161"/>
       <c r="CQ32" s="63"/>
       <c r="CR32" s="63"/>
       <c r="CS32" s="63"/>
-      <c r="CT32" s="63"/>
+      <c r="CT32" s="179"/>
       <c r="CU32" s="59"/>
       <c r="CV32" s="59"/>
       <c r="CW32" s="59"/>
@@ -6591,17 +6732,17 @@
       <c r="CG33" s="82"/>
       <c r="CH33" s="82"/>
       <c r="CI33" s="82"/>
-      <c r="CJ33" s="82"/>
-      <c r="CK33" s="82"/>
+      <c r="CJ33" s="174"/>
+      <c r="CK33" s="162"/>
       <c r="CL33" s="82"/>
       <c r="CM33" s="82"/>
       <c r="CN33" s="82"/>
       <c r="CO33" s="82"/>
-      <c r="CP33" s="82"/>
+      <c r="CP33" s="162"/>
       <c r="CQ33" s="82"/>
       <c r="CR33" s="82"/>
       <c r="CS33" s="82"/>
-      <c r="CT33" s="82"/>
+      <c r="CT33" s="174"/>
       <c r="CU33" s="82"/>
       <c r="CV33" s="82"/>
       <c r="CW33" s="82"/>
@@ -6727,17 +6868,17 @@
       <c r="CG34" s="79"/>
       <c r="CH34" s="79"/>
       <c r="CI34" s="79"/>
-      <c r="CJ34" s="79"/>
-      <c r="CK34" s="71"/>
+      <c r="CJ34" s="173"/>
+      <c r="CK34" s="182"/>
       <c r="CL34" s="71"/>
       <c r="CM34" s="71"/>
       <c r="CN34" s="71"/>
       <c r="CO34" s="71"/>
-      <c r="CP34" s="79"/>
+      <c r="CP34" s="161"/>
       <c r="CQ34" s="93"/>
       <c r="CR34" s="93"/>
       <c r="CS34" s="93"/>
-      <c r="CT34" s="93"/>
+      <c r="CT34" s="181"/>
       <c r="CU34" s="71"/>
       <c r="CV34" s="71"/>
       <c r="CW34" s="71"/>
@@ -6850,17 +6991,17 @@
       <c r="CG35" s="24"/>
       <c r="CH35" s="24"/>
       <c r="CI35" s="24"/>
-      <c r="CJ35" s="24"/>
-      <c r="CK35" s="24"/>
+      <c r="CJ35" s="167"/>
+      <c r="CK35" s="156"/>
       <c r="CL35" s="24"/>
       <c r="CM35" s="24"/>
       <c r="CN35" s="24"/>
       <c r="CO35" s="24"/>
-      <c r="CP35" s="24"/>
+      <c r="CP35" s="156"/>
       <c r="CQ35" s="93"/>
       <c r="CR35" s="93"/>
       <c r="CS35" s="93"/>
-      <c r="CT35" s="93"/>
+      <c r="CT35" s="181"/>
       <c r="CU35" s="71"/>
       <c r="CV35" s="71"/>
       <c r="CW35" s="71"/>
@@ -6986,17 +7127,17 @@
       <c r="CG36" s="79"/>
       <c r="CH36" s="79"/>
       <c r="CI36" s="79"/>
-      <c r="CJ36" s="79"/>
-      <c r="CK36" s="71"/>
+      <c r="CJ36" s="173"/>
+      <c r="CK36" s="182"/>
       <c r="CL36" s="71"/>
       <c r="CM36" s="71"/>
       <c r="CN36" s="71"/>
       <c r="CO36" s="71"/>
-      <c r="CP36" s="79"/>
+      <c r="CP36" s="161"/>
       <c r="CQ36" s="93"/>
       <c r="CR36" s="93"/>
       <c r="CS36" s="93"/>
-      <c r="CT36" s="93"/>
+      <c r="CT36" s="181"/>
       <c r="CU36" s="71"/>
       <c r="CV36" s="71"/>
       <c r="CW36" s="71"/>
@@ -7122,17 +7263,17 @@
       <c r="CG37" s="79"/>
       <c r="CH37" s="79"/>
       <c r="CI37" s="79"/>
-      <c r="CJ37" s="79"/>
-      <c r="CK37" s="71"/>
+      <c r="CJ37" s="173"/>
+      <c r="CK37" s="182"/>
       <c r="CL37" s="71"/>
       <c r="CM37" s="71"/>
       <c r="CN37" s="71"/>
       <c r="CO37" s="71"/>
-      <c r="CP37" s="79"/>
+      <c r="CP37" s="161"/>
       <c r="CQ37" s="93"/>
       <c r="CR37" s="93"/>
       <c r="CS37" s="93"/>
-      <c r="CT37" s="93"/>
+      <c r="CT37" s="181"/>
       <c r="CU37" s="71"/>
       <c r="CV37" s="71"/>
       <c r="CW37" s="71"/>
@@ -7247,17 +7388,17 @@
       <c r="CG38" s="74"/>
       <c r="CH38" s="74"/>
       <c r="CI38" s="74"/>
-      <c r="CJ38" s="74"/>
-      <c r="CK38" s="74"/>
+      <c r="CJ38" s="171"/>
+      <c r="CK38" s="159"/>
       <c r="CL38" s="74"/>
       <c r="CM38" s="74"/>
       <c r="CN38" s="74"/>
       <c r="CO38" s="74"/>
-      <c r="CP38" s="74"/>
+      <c r="CP38" s="159"/>
       <c r="CQ38" s="74"/>
       <c r="CR38" s="74"/>
       <c r="CS38" s="74"/>
-      <c r="CT38" s="74"/>
+      <c r="CT38" s="171"/>
       <c r="CU38" s="74"/>
       <c r="CV38" s="74"/>
       <c r="CW38" s="74"/>
@@ -7383,17 +7524,17 @@
       <c r="CG39" s="24"/>
       <c r="CH39" s="24"/>
       <c r="CI39" s="24"/>
-      <c r="CJ39" s="24"/>
-      <c r="CK39" s="59"/>
+      <c r="CJ39" s="167"/>
+      <c r="CK39" s="163"/>
       <c r="CL39" s="59"/>
       <c r="CM39" s="59"/>
       <c r="CN39" s="59"/>
       <c r="CO39" s="59"/>
-      <c r="CP39" s="62"/>
+      <c r="CP39" s="158"/>
       <c r="CQ39" s="63"/>
       <c r="CR39" s="63"/>
       <c r="CS39" s="63"/>
-      <c r="CT39" s="63"/>
+      <c r="CT39" s="179"/>
       <c r="CU39" s="59"/>
       <c r="CV39" s="59"/>
       <c r="CW39" s="59"/>
@@ -7518,17 +7659,17 @@
       <c r="CG40" s="24"/>
       <c r="CH40" s="24"/>
       <c r="CI40" s="24"/>
-      <c r="CJ40" s="24"/>
-      <c r="CK40" s="24"/>
+      <c r="CJ40" s="167"/>
+      <c r="CK40" s="156"/>
       <c r="CL40" s="24"/>
       <c r="CM40" s="24"/>
       <c r="CN40" s="24"/>
       <c r="CO40" s="24"/>
-      <c r="CP40" s="62"/>
+      <c r="CP40" s="158"/>
       <c r="CQ40" s="63"/>
       <c r="CR40" s="63"/>
       <c r="CS40" s="63"/>
-      <c r="CT40" s="63"/>
+      <c r="CT40" s="179"/>
       <c r="CU40" s="59"/>
       <c r="CV40" s="59"/>
       <c r="CW40" s="59"/>
@@ -7643,17 +7784,17 @@
       <c r="CG41" s="74"/>
       <c r="CH41" s="74"/>
       <c r="CI41" s="74"/>
-      <c r="CJ41" s="74"/>
-      <c r="CK41" s="74"/>
+      <c r="CJ41" s="171"/>
+      <c r="CK41" s="159"/>
       <c r="CL41" s="74"/>
       <c r="CM41" s="74"/>
       <c r="CN41" s="74"/>
       <c r="CO41" s="74"/>
-      <c r="CP41" s="74"/>
+      <c r="CP41" s="159"/>
       <c r="CQ41" s="74"/>
       <c r="CR41" s="74"/>
       <c r="CS41" s="74"/>
-      <c r="CT41" s="74"/>
+      <c r="CT41" s="171"/>
       <c r="CU41" s="74"/>
       <c r="CV41" s="74"/>
       <c r="CW41" s="74"/>
@@ -7779,17 +7920,17 @@
       <c r="CG42" s="59"/>
       <c r="CH42" s="59"/>
       <c r="CI42" s="59"/>
-      <c r="CJ42" s="59"/>
-      <c r="CK42" s="59"/>
+      <c r="CJ42" s="175"/>
+      <c r="CK42" s="163"/>
       <c r="CL42" s="59"/>
       <c r="CM42" s="59"/>
       <c r="CN42" s="59"/>
       <c r="CO42" s="59"/>
-      <c r="CP42" s="62"/>
+      <c r="CP42" s="158"/>
       <c r="CQ42" s="63"/>
       <c r="CR42" s="63"/>
       <c r="CS42" s="63"/>
-      <c r="CT42" s="63"/>
+      <c r="CT42" s="179"/>
       <c r="CU42" s="59"/>
       <c r="CV42" s="59"/>
       <c r="CW42" s="59"/>
@@ -7915,17 +8056,17 @@
       <c r="CG43" s="24"/>
       <c r="CH43" s="24"/>
       <c r="CI43" s="24"/>
-      <c r="CJ43" s="24"/>
-      <c r="CK43" s="24"/>
+      <c r="CJ43" s="167"/>
+      <c r="CK43" s="156"/>
       <c r="CL43" s="24"/>
       <c r="CM43" s="24"/>
       <c r="CN43" s="24"/>
       <c r="CO43" s="24"/>
-      <c r="CP43" s="62"/>
+      <c r="CP43" s="158"/>
       <c r="CQ43" s="63"/>
       <c r="CR43" s="63"/>
       <c r="CS43" s="63"/>
-      <c r="CT43" s="63"/>
+      <c r="CT43" s="179"/>
       <c r="CU43" s="59"/>
       <c r="CV43" s="59"/>
       <c r="CW43" s="59"/>
@@ -8040,17 +8181,17 @@
       <c r="CG44" s="74"/>
       <c r="CH44" s="74"/>
       <c r="CI44" s="74"/>
-      <c r="CJ44" s="74"/>
-      <c r="CK44" s="74"/>
+      <c r="CJ44" s="171"/>
+      <c r="CK44" s="159"/>
       <c r="CL44" s="74"/>
       <c r="CM44" s="74"/>
       <c r="CN44" s="74"/>
       <c r="CO44" s="74"/>
-      <c r="CP44" s="74"/>
+      <c r="CP44" s="159"/>
       <c r="CQ44" s="74"/>
       <c r="CR44" s="74"/>
       <c r="CS44" s="74"/>
-      <c r="CT44" s="74"/>
+      <c r="CT44" s="171"/>
       <c r="CU44" s="74"/>
       <c r="CV44" s="74"/>
       <c r="CW44" s="74"/>
@@ -8176,17 +8317,17 @@
       <c r="CG45" s="62"/>
       <c r="CH45" s="62"/>
       <c r="CI45" s="62"/>
-      <c r="CJ45" s="62"/>
-      <c r="CK45" s="24"/>
+      <c r="CJ45" s="170"/>
+      <c r="CK45" s="156"/>
       <c r="CL45" s="24"/>
       <c r="CM45" s="24"/>
       <c r="CN45" s="24"/>
       <c r="CO45" s="24"/>
-      <c r="CP45" s="24"/>
+      <c r="CP45" s="156"/>
       <c r="CQ45" s="63"/>
       <c r="CR45" s="63"/>
       <c r="CS45" s="63"/>
-      <c r="CT45" s="63"/>
+      <c r="CT45" s="179"/>
       <c r="CU45" s="59"/>
       <c r="CV45" s="59"/>
       <c r="CW45" s="59"/>
@@ -8312,17 +8453,17 @@
       <c r="CG46" s="62"/>
       <c r="CH46" s="62"/>
       <c r="CI46" s="62"/>
-      <c r="CJ46" s="62"/>
-      <c r="CK46" s="59"/>
+      <c r="CJ46" s="170"/>
+      <c r="CK46" s="163"/>
       <c r="CL46" s="59"/>
       <c r="CM46" s="59"/>
       <c r="CN46" s="59"/>
       <c r="CO46" s="59"/>
-      <c r="CP46" s="62"/>
+      <c r="CP46" s="158"/>
       <c r="CQ46" s="63"/>
       <c r="CR46" s="63"/>
       <c r="CS46" s="63"/>
-      <c r="CT46" s="63"/>
+      <c r="CT46" s="179"/>
       <c r="CU46" s="59"/>
       <c r="CV46" s="59"/>
       <c r="CW46" s="59"/>
@@ -8433,17 +8574,17 @@
       <c r="CG47" s="1"/>
       <c r="CH47" s="1"/>
       <c r="CI47" s="1"/>
-      <c r="CJ47" s="1"/>
-      <c r="CK47" s="1"/>
+      <c r="CJ47" s="165"/>
+      <c r="CK47" s="154"/>
       <c r="CL47" s="1"/>
       <c r="CM47" s="1"/>
       <c r="CN47" s="1"/>
       <c r="CO47" s="1"/>
-      <c r="CP47" s="1"/>
+      <c r="CP47" s="154"/>
       <c r="CQ47" s="1"/>
       <c r="CR47" s="1"/>
       <c r="CS47" s="1"/>
-      <c r="CT47" s="1"/>
+      <c r="CT47" s="165"/>
       <c r="CU47" s="1"/>
       <c r="CV47" s="1"/>
       <c r="CW47" s="1"/>
@@ -8468,106 +8609,106 @@
     </row>
     <row r="48" spans="1:119" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-      <c r="B48" s="145" t="str">
+      <c r="B48" s="122" t="str">
         <f>HYPERLINK("https://goo.gl/L6X1St","CLICK HERE TO CREATE PROJECT TIMELINE TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE PROJECT TIMELINE TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C48" s="146"/>
-      <c r="D48" s="146"/>
-      <c r="E48" s="146"/>
-      <c r="F48" s="146"/>
-      <c r="G48" s="146"/>
-      <c r="H48" s="146"/>
-      <c r="I48" s="146"/>
-      <c r="J48" s="146"/>
-      <c r="K48" s="146"/>
-      <c r="L48" s="146"/>
-      <c r="M48" s="146"/>
-      <c r="N48" s="146"/>
-      <c r="O48" s="146"/>
-      <c r="P48" s="146"/>
-      <c r="Q48" s="146"/>
-      <c r="R48" s="146"/>
-      <c r="S48" s="146"/>
-      <c r="T48" s="146"/>
-      <c r="U48" s="146"/>
-      <c r="V48" s="146"/>
-      <c r="W48" s="146"/>
-      <c r="X48" s="146"/>
-      <c r="Y48" s="146"/>
-      <c r="Z48" s="146"/>
-      <c r="AA48" s="146"/>
-      <c r="AB48" s="146"/>
-      <c r="AC48" s="146"/>
-      <c r="AD48" s="146"/>
-      <c r="AE48" s="146"/>
-      <c r="AF48" s="146"/>
-      <c r="AG48" s="146"/>
-      <c r="AH48" s="146"/>
-      <c r="AI48" s="146"/>
-      <c r="AJ48" s="146"/>
-      <c r="AK48" s="146"/>
-      <c r="AL48" s="146"/>
-      <c r="AM48" s="146"/>
-      <c r="AN48" s="146"/>
-      <c r="AO48" s="146"/>
-      <c r="AP48" s="146"/>
-      <c r="AQ48" s="146"/>
-      <c r="AR48" s="146"/>
-      <c r="AS48" s="146"/>
-      <c r="AT48" s="146"/>
-      <c r="AU48" s="146"/>
-      <c r="AV48" s="146"/>
-      <c r="AW48" s="146"/>
-      <c r="AX48" s="146"/>
-      <c r="AY48" s="146"/>
-      <c r="AZ48" s="146"/>
-      <c r="BA48" s="146"/>
-      <c r="BB48" s="146"/>
-      <c r="BC48" s="146"/>
-      <c r="BD48" s="146"/>
-      <c r="BE48" s="146"/>
-      <c r="BF48" s="146"/>
-      <c r="BG48" s="146"/>
-      <c r="BH48" s="146"/>
-      <c r="BI48" s="146"/>
-      <c r="BJ48" s="146"/>
-      <c r="BK48" s="146"/>
-      <c r="BL48" s="146"/>
-      <c r="BM48" s="146"/>
-      <c r="BN48" s="146"/>
-      <c r="BO48" s="146"/>
-      <c r="BP48" s="146"/>
-      <c r="BQ48" s="146"/>
-      <c r="BR48" s="146"/>
-      <c r="BS48" s="146"/>
-      <c r="BT48" s="146"/>
-      <c r="BU48" s="146"/>
-      <c r="BV48" s="146"/>
-      <c r="BW48" s="146"/>
-      <c r="BX48" s="146"/>
-      <c r="BY48" s="146"/>
-      <c r="BZ48" s="146"/>
-      <c r="CA48" s="146"/>
-      <c r="CB48" s="146"/>
-      <c r="CC48" s="146"/>
-      <c r="CD48" s="146"/>
-      <c r="CE48" s="146"/>
-      <c r="CF48" s="146"/>
-      <c r="CG48" s="146"/>
-      <c r="CH48" s="146"/>
-      <c r="CI48" s="146"/>
-      <c r="CJ48" s="146"/>
-      <c r="CK48" s="146"/>
-      <c r="CL48" s="146"/>
-      <c r="CM48" s="146"/>
-      <c r="CN48" s="146"/>
-      <c r="CO48" s="147"/>
-      <c r="CP48" s="1"/>
+      <c r="C48" s="123"/>
+      <c r="D48" s="123"/>
+      <c r="E48" s="123"/>
+      <c r="F48" s="123"/>
+      <c r="G48" s="123"/>
+      <c r="H48" s="123"/>
+      <c r="I48" s="123"/>
+      <c r="J48" s="123"/>
+      <c r="K48" s="123"/>
+      <c r="L48" s="123"/>
+      <c r="M48" s="123"/>
+      <c r="N48" s="123"/>
+      <c r="O48" s="123"/>
+      <c r="P48" s="123"/>
+      <c r="Q48" s="123"/>
+      <c r="R48" s="123"/>
+      <c r="S48" s="123"/>
+      <c r="T48" s="123"/>
+      <c r="U48" s="123"/>
+      <c r="V48" s="123"/>
+      <c r="W48" s="123"/>
+      <c r="X48" s="123"/>
+      <c r="Y48" s="123"/>
+      <c r="Z48" s="123"/>
+      <c r="AA48" s="123"/>
+      <c r="AB48" s="123"/>
+      <c r="AC48" s="123"/>
+      <c r="AD48" s="123"/>
+      <c r="AE48" s="123"/>
+      <c r="AF48" s="123"/>
+      <c r="AG48" s="123"/>
+      <c r="AH48" s="123"/>
+      <c r="AI48" s="123"/>
+      <c r="AJ48" s="123"/>
+      <c r="AK48" s="123"/>
+      <c r="AL48" s="123"/>
+      <c r="AM48" s="123"/>
+      <c r="AN48" s="123"/>
+      <c r="AO48" s="123"/>
+      <c r="AP48" s="123"/>
+      <c r="AQ48" s="123"/>
+      <c r="AR48" s="123"/>
+      <c r="AS48" s="123"/>
+      <c r="AT48" s="123"/>
+      <c r="AU48" s="123"/>
+      <c r="AV48" s="123"/>
+      <c r="AW48" s="123"/>
+      <c r="AX48" s="123"/>
+      <c r="AY48" s="123"/>
+      <c r="AZ48" s="123"/>
+      <c r="BA48" s="123"/>
+      <c r="BB48" s="123"/>
+      <c r="BC48" s="123"/>
+      <c r="BD48" s="123"/>
+      <c r="BE48" s="123"/>
+      <c r="BF48" s="123"/>
+      <c r="BG48" s="123"/>
+      <c r="BH48" s="123"/>
+      <c r="BI48" s="123"/>
+      <c r="BJ48" s="123"/>
+      <c r="BK48" s="123"/>
+      <c r="BL48" s="123"/>
+      <c r="BM48" s="123"/>
+      <c r="BN48" s="123"/>
+      <c r="BO48" s="123"/>
+      <c r="BP48" s="123"/>
+      <c r="BQ48" s="123"/>
+      <c r="BR48" s="123"/>
+      <c r="BS48" s="123"/>
+      <c r="BT48" s="123"/>
+      <c r="BU48" s="123"/>
+      <c r="BV48" s="123"/>
+      <c r="BW48" s="123"/>
+      <c r="BX48" s="123"/>
+      <c r="BY48" s="123"/>
+      <c r="BZ48" s="123"/>
+      <c r="CA48" s="123"/>
+      <c r="CB48" s="123"/>
+      <c r="CC48" s="123"/>
+      <c r="CD48" s="123"/>
+      <c r="CE48" s="123"/>
+      <c r="CF48" s="123"/>
+      <c r="CG48" s="123"/>
+      <c r="CH48" s="123"/>
+      <c r="CI48" s="123"/>
+      <c r="CJ48" s="123"/>
+      <c r="CK48" s="123"/>
+      <c r="CL48" s="123"/>
+      <c r="CM48" s="123"/>
+      <c r="CN48" s="123"/>
+      <c r="CO48" s="124"/>
+      <c r="CP48" s="154"/>
       <c r="CQ48" s="1"/>
       <c r="CR48" s="1"/>
       <c r="CS48" s="1"/>
-      <c r="CT48" s="1"/>
+      <c r="CT48" s="165"/>
       <c r="CU48" s="1"/>
       <c r="CV48" s="1"/>
       <c r="CW48" s="1"/>
@@ -8678,17 +8819,17 @@
       <c r="CG49" s="1"/>
       <c r="CH49" s="1"/>
       <c r="CI49" s="1"/>
-      <c r="CJ49" s="1"/>
-      <c r="CK49" s="1"/>
+      <c r="CJ49" s="165"/>
+      <c r="CK49" s="154"/>
       <c r="CL49" s="1"/>
       <c r="CM49" s="1"/>
       <c r="CN49" s="1"/>
       <c r="CO49" s="1"/>
-      <c r="CP49" s="1"/>
+      <c r="CP49" s="154"/>
       <c r="CQ49" s="1"/>
       <c r="CR49" s="1"/>
       <c r="CS49" s="1"/>
-      <c r="CT49" s="1"/>
+      <c r="CT49" s="165"/>
       <c r="CU49" s="1"/>
       <c r="CV49" s="1"/>
       <c r="CW49" s="1"/>
@@ -9721,6 +9862,32 @@
     <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="AI2:AV2"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="I5:Q5"/>
+    <mergeCell ref="R5:AV5"/>
+    <mergeCell ref="I4:Q4"/>
+    <mergeCell ref="R4:AV4"/>
+    <mergeCell ref="I7:AB7"/>
+    <mergeCell ref="N8:R8"/>
+    <mergeCell ref="X8:AB8"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="AH8:AL8"/>
+    <mergeCell ref="AC8:AG8"/>
+    <mergeCell ref="AW8:BA8"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="AC7:BA7"/>
+    <mergeCell ref="CU7:DN7"/>
+    <mergeCell ref="BV7:CT7"/>
+    <mergeCell ref="BL8:BP8"/>
+    <mergeCell ref="BB7:BU7"/>
+    <mergeCell ref="CP8:CT8"/>
+    <mergeCell ref="DJ8:DN8"/>
+    <mergeCell ref="CU8:CY8"/>
+    <mergeCell ref="CZ8:DD8"/>
+    <mergeCell ref="DE8:DI8"/>
     <mergeCell ref="B48:CO48"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="S8:W8"/>
@@ -9737,32 +9904,6 @@
     <mergeCell ref="BV8:BZ8"/>
     <mergeCell ref="BQ8:BU8"/>
     <mergeCell ref="BG8:BK8"/>
-    <mergeCell ref="AW8:BA8"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="AC7:BA7"/>
-    <mergeCell ref="CU7:DN7"/>
-    <mergeCell ref="BV7:CT7"/>
-    <mergeCell ref="BL8:BP8"/>
-    <mergeCell ref="BB7:BU7"/>
-    <mergeCell ref="CP8:CT8"/>
-    <mergeCell ref="DJ8:DN8"/>
-    <mergeCell ref="CU8:CY8"/>
-    <mergeCell ref="CZ8:DD8"/>
-    <mergeCell ref="DE8:DI8"/>
-    <mergeCell ref="AI2:AV2"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="I5:Q5"/>
-    <mergeCell ref="R5:AV5"/>
-    <mergeCell ref="I4:Q4"/>
-    <mergeCell ref="R4:AV4"/>
-    <mergeCell ref="I7:AB7"/>
-    <mergeCell ref="N8:R8"/>
-    <mergeCell ref="X8:AB8"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="AH8:AL8"/>
-    <mergeCell ref="AC8:AG8"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:H10 H12:H46">
     <cfRule type="colorScale" priority="1">

</xml_diff>